<commit_message>
Veel opmaakwijzigingen. Correctie foutjes. Excelbestand levensonderhoud uitgebreid met query.
</commit_message>
<xml_diff>
--- a/resources/screendumps.xlsx
+++ b/resources/screendumps.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\studieboeken\excelanalyse-quarto\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\studieboeken\excelanalyse\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D42AEF-9AE4-4546-96D7-C1E567C0C2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2C2775-C7D3-4C53-890B-5A4D45B92B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CEF6CC8B-8057-4304-BA4D-80104F4CB2BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{CEF6CC8B-8057-4304-BA4D-80104F4CB2BC}"/>
   </bookViews>
   <sheets>
     <sheet name="x-y" sheetId="1" r:id="rId1"/>
     <sheet name="studietijd-cijfer" sheetId="2" r:id="rId2"/>
+    <sheet name="oef2_1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>x</t>
   </si>
@@ -50,6 +51,66 @@
   <si>
     <t>cijfer</t>
   </si>
+  <si>
+    <t>voornaam</t>
+  </si>
+  <si>
+    <t>geslacht</t>
+  </si>
+  <si>
+    <t>haarkleur</t>
+  </si>
+  <si>
+    <t>lengte</t>
+  </si>
+  <si>
+    <t>gewicht</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Mari</t>
+  </si>
+  <si>
+    <t>Otto</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Vicky</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>bruin</t>
+  </si>
+  <si>
+    <t>blond</t>
+  </si>
+  <si>
+    <t>zwart</t>
+  </si>
+  <si>
+    <t>rood</t>
+  </si>
+  <si>
+    <t>groot</t>
+  </si>
+  <si>
+    <t>normaal</t>
+  </si>
+  <si>
+    <t>klein</t>
+  </si>
+  <si>
+    <t>iq</t>
+  </si>
 </sst>
 </file>
 
@@ -58,8 +119,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,11 +156,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -982,7 +1057,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1014,7 +1089,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -2315,9 +2390,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2355,7 +2430,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2461,7 +2536,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2603,7 +2678,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2617,13 +2692,13 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="1" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2631,7 +2706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -2639,7 +2714,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1.5</v>
       </c>
@@ -2647,7 +2722,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -2655,7 +2730,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2.9</v>
       </c>
@@ -2663,7 +2738,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3.1</v>
       </c>
@@ -2671,7 +2746,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>3.8</v>
       </c>
@@ -2679,7 +2754,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -2687,7 +2762,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>4.9000000000000004</v>
       </c>
@@ -2695,7 +2770,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>6.3</v>
       </c>
@@ -2703,7 +2778,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>6.9</v>
       </c>
@@ -2711,7 +2786,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>7.8</v>
       </c>
@@ -2719,7 +2794,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>8.5</v>
       </c>
@@ -2727,7 +2802,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>9.4</v>
       </c>
@@ -2735,7 +2810,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -2743,7 +2818,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>9.8000000000000007</v>
       </c>
@@ -2761,13 +2836,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CADBF0-5240-4FFE-B8A5-0537E2451A72}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2775,7 +2850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>6</v>
       </c>
@@ -2783,7 +2858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>8</v>
       </c>
@@ -2791,7 +2866,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2799,7 +2874,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2807,7 +2882,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -2815,7 +2890,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>11</v>
       </c>
@@ -2823,7 +2898,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
@@ -2831,7 +2906,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2839,7 +2914,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2847,7 +2922,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>12</v>
       </c>
@@ -2855,7 +2930,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2863,7 +2938,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
@@ -2871,7 +2946,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2879,7 +2954,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -2887,7 +2962,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2895,7 +2970,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>9</v>
       </c>
@@ -2903,7 +2978,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2911,7 +2986,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2919,7 +2994,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10</v>
       </c>
@@ -2927,7 +3002,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>9</v>
       </c>
@@ -2939,4 +3014,139 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA05D0D-B8CA-4014-825D-F79906E74CDD}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4">
+        <v>185</v>
+      </c>
+      <c r="F2" s="4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4">
+        <v>176</v>
+      </c>
+      <c r="F3" s="4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4">
+        <v>181</v>
+      </c>
+      <c r="F4" s="4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4">
+        <v>178</v>
+      </c>
+      <c r="F5" s="4">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4">
+        <v>164</v>
+      </c>
+      <c r="F6" s="4">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>